<commit_message>
Added Search sheet in Test Data file
</commit_message>
<xml_diff>
--- a/Flipkart_Automation/TestData/Data.xlsx
+++ b/Flipkart_Automation/TestData/Data.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="Search" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -411,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -511,4 +512,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>